<commit_message>
PROD Suite Update for TC 4,8 and 12
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/Prod/ALL_PAGES/END_TO_END/TC04_SearchCategory.xlsx
+++ b/Input_files/Actual_testcases/Kaman/Prod/ALL_PAGES/END_TO_END/TC04_SearchCategory.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Vaibhav Oza\KAMAN_ECTEST_IE_SANITY-master\Input_files\Actual_testcases\Kaman\Prod\ALL_PAGES\END_TO_END\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
@@ -10,7 +15,7 @@
     <sheet name="TC04_SearchCategory" sheetId="1" r:id="rId1"/>
     <sheet name="Testdata" sheetId="12" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" calcOnSave="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -23,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
   <si>
     <t>TestCase</t>
   </si>
@@ -55,88 +60,100 @@
     <t>VERIFY_WEBELEMENT_PRESENT</t>
   </si>
   <si>
+    <t>Uname</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>bep-dvlp@kaman.com</t>
+  </si>
+  <si>
+    <t>bep999</t>
+  </si>
+  <si>
+    <t>AccModel</t>
+  </si>
+  <si>
+    <t>Welcomeelement</t>
+  </si>
+  <si>
+    <t>MyaccountSection</t>
+  </si>
+  <si>
+    <t>GearingPLPHeader</t>
+  </si>
+  <si>
+    <t>CategoryFilter</t>
+  </si>
+  <si>
+    <t>Gearing</t>
+  </si>
+  <si>
+    <t>PLPpageTitle</t>
+  </si>
+  <si>
+    <t>PLPAddtocart</t>
+  </si>
+  <si>
+    <t>PDPAddtoCart</t>
+  </si>
+  <si>
+    <t>PDPProductHeader</t>
+  </si>
+  <si>
+    <t>PDPBreadcrumbs</t>
+  </si>
+  <si>
+    <t>$BaseURL</t>
+  </si>
+  <si>
+    <t>CSS</t>
+  </si>
+  <si>
+    <t>EleType1</t>
+  </si>
+  <si>
+    <t>EleType2</t>
+  </si>
+  <si>
+    <t>JSElement</t>
+  </si>
+  <si>
+    <t>TC04_SearchCategory</t>
+  </si>
+  <si>
+    <t>CLICK_PRE_ENTERTEXT</t>
+  </si>
+  <si>
+    <t>SearchBoxHomePage</t>
+  </si>
+  <si>
+    <t>ENTERTEXT</t>
+  </si>
+  <si>
+    <t>validSearch</t>
+  </si>
+  <si>
+    <t>PRESS_ENTER</t>
+  </si>
+  <si>
+    <t>WAIT</t>
+  </si>
+  <si>
     <t>VERIFY_TEXT_PRESENT</t>
   </si>
   <si>
-    <t>Uname</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>CLICK</t>
-  </si>
-  <si>
-    <t>bep-dvlp@kaman.com</t>
-  </si>
-  <si>
-    <t>bep999</t>
-  </si>
-  <si>
-    <t>AccModel</t>
-  </si>
-  <si>
-    <t>Welcomeelement</t>
-  </si>
-  <si>
-    <t>MyaccountSection</t>
-  </si>
-  <si>
-    <t>MOUSEOVER</t>
-  </si>
-  <si>
-    <t>GearingPLPHeader</t>
-  </si>
-  <si>
-    <t>CategoryFilter</t>
-  </si>
-  <si>
-    <t>Gearing</t>
+    <t>GearingCategoryHeader</t>
   </si>
   <si>
     <t>VERIFY_PAGE_TITLE</t>
   </si>
   <si>
-    <t>PLPpageTitle</t>
-  </si>
-  <si>
-    <t>ProductMegamenu</t>
-  </si>
-  <si>
-    <t>Gearing | KamanDirect</t>
-  </si>
-  <si>
-    <t>GearingCategoryHeader</t>
-  </si>
-  <si>
-    <t>PLPAddtocart</t>
-  </si>
-  <si>
-    <t>PDPAddtoCart</t>
-  </si>
-  <si>
-    <t>PDPProductHeader</t>
-  </si>
-  <si>
-    <t>PDPBreadcrumbs</t>
-  </si>
-  <si>
-    <t>$BaseURL</t>
-  </si>
-  <si>
-    <t>CSS</t>
-  </si>
-  <si>
-    <t>EleType1</t>
-  </si>
-  <si>
-    <t>EleType2</t>
-  </si>
-  <si>
-    <t>JSElement</t>
-  </si>
-  <si>
-    <t>TC04_SearchCategory</t>
+    <t>Gear Racks and Pinions</t>
+  </si>
+  <si>
+    <t>Gear Racks and Pinions | Kaman Industrial</t>
   </si>
 </sst>
 </file>
@@ -552,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -585,8 +602,8 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>37</v>
+      <c r="A2" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
@@ -600,68 +617,137 @@
     <row r="3" spans="1:5">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>33</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3"/>
-      <c r="B4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>33</v>
-      </c>
+      <c r="B4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3"/>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
+      <c r="B5" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>20</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3"/>
-      <c r="B6" s="4" t="s">
-        <v>9</v>
+      <c r="B6" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
-        <v>24</v>
+        <v>35</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="3"/>
+      <c r="B13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -673,16 +759,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:B16"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -698,28 +784,28 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="b">
         <v>1</v>
@@ -727,7 +813,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3" t="b">
         <v>1</v>
@@ -735,7 +821,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3" t="b">
         <v>1</v>
@@ -743,15 +829,15 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B9" s="3" t="b">
         <v>1</v>
@@ -759,15 +845,15 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B11" s="3" t="b">
         <v>1</v>
@@ -775,7 +861,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B12" s="3" t="b">
         <v>1</v>
@@ -783,7 +869,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B13" s="3" t="b">
         <v>1</v>
@@ -791,7 +877,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B14" s="3" t="b">
         <v>1</v>
@@ -799,18 +885,26 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="3" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>36</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -823,18 +917,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1035,6 +1129,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -1047,14 +1149,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>